<commit_message>
CE09OSPM added eng bar codes and bogey for D4 recovery date
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE09OSPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_CE09OSPM_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CE_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="12720" windowHeight="12408" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -23,24 +23,24 @@
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0_0">Moorings!$B$1:$K$84</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$399</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$398</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$399</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$H$399</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$H$398</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$H$398</definedName>
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$H$1</definedName>
-    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$H$399</definedName>
+    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$H$398</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$H$29</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$H$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$84</definedName>
-    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$399</definedName>
+    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$398</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>Ref Des</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Located in the calibration certificate for QSP-2200, under Calibration Factors, after Wet (Volts/(quanta/cm2-sec))</t>
-  </si>
-  <si>
-    <t>CE09OSPM-SBS01-00-RTE000000</t>
   </si>
   <si>
     <t>CE09OSPM-WFP01-00-WFPENG000</t>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>A00285</t>
+  </si>
+  <si>
+    <t>OL000372</t>
   </si>
 </sst>
 </file>
@@ -982,30 +982,30 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875"/>
-    <col min="3" max="3" width="39.44140625"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.44140625"/>
-    <col min="8" max="8" width="18.6640625"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875"/>
-    <col min="11" max="11" width="12.6640625"/>
-    <col min="12" max="12" width="51.6640625"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875"/>
+    <col min="3" max="3" width="39.42578125"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125"/>
+    <col min="8" max="8" width="18.7109375"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875"/>
+    <col min="11" max="11" width="12.7109375"/>
+    <col min="12" max="12" width="51.7109375"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="1027" width="8.6640625"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="1027" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.6">
+    <row r="1" spans="1:14" ht="25.5">
       <c r="A1" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -1041,9 +1041,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6">
+    <row r="2" spans="1:14" ht="15.75">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>34</v>
@@ -1064,10 +1064,10 @@
         <v>41866</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="J2" s="2">
         <v>536.1</v>
@@ -1101,37 +1101,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="58.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625"/>
-    <col min="11" max="11" width="11.88671875"/>
-    <col min="12" max="12" width="14.44140625"/>
-    <col min="13" max="13" width="13.44140625"/>
-    <col min="14" max="1028" width="8.6640625"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125"/>
+    <col min="11" max="11" width="11.85546875"/>
+    <col min="12" max="12" width="14.42578125"/>
+    <col min="13" max="13" width="13.42578125"/>
+    <col min="14" max="1028" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6">
+    <row r="1" spans="1:9" ht="25.5">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>10</v>
@@ -1140,7 +1140,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>11</v>
@@ -1157,7 +1157,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>40</v>
@@ -1166,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>16</v>
@@ -1186,7 +1186,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -1195,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -1213,7 +1213,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>40</v>
@@ -1222,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>15</v>
@@ -1240,7 +1240,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -1249,10 +1249,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>17</v>
@@ -1269,7 +1269,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>40</v>
@@ -1278,10 +1278,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>18</v>
@@ -1298,7 +1298,7 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>40</v>
@@ -1307,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>19</v>
@@ -1327,7 +1327,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>40</v>
@@ -1336,10 +1336,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>20</v>
@@ -1356,7 +1356,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>40</v>
@@ -1365,10 +1365,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>21</v>
@@ -1395,7 +1395,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>40</v>
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="5">
         <v>110</v>
@@ -1421,7 +1421,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>40</v>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="5">
         <v>110</v>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>40</v>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="6">
         <v>100014</v>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>40</v>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="6">
         <v>100014</v>
@@ -1519,7 +1519,7 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>40</v>
@@ -1528,19 +1528,19 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="5">
         <v>1030</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="19">
         <v>1.0760000000000001</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1548,7 +1548,7 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>40</v>
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="5">
         <v>1030</v>
@@ -1577,7 +1577,7 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>40</v>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="5">
         <v>1030</v>
@@ -1598,7 +1598,7 @@
         <v>51</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1606,7 +1606,7 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>40</v>
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="5">
         <v>1030</v>
@@ -1635,7 +1635,7 @@
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>40</v>
@@ -1644,13 +1644,13 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="5">
         <v>1030</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="19">
         <v>3.9E-2</v>
@@ -1664,7 +1664,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>40</v>
@@ -1673,13 +1673,13 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="5">
         <v>1030</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" s="19">
         <v>700</v>
@@ -1693,7 +1693,7 @@
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>40</v>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="5">
         <v>1030</v>
@@ -1722,7 +1722,7 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>40</v>
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="5">
         <v>1030</v>
@@ -1751,7 +1751,7 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>40</v>
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="5">
         <v>1030</v>
@@ -1780,7 +1780,7 @@
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>40</v>
@@ -1789,13 +1789,13 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" s="5">
         <v>1030</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="19">
         <v>124</v>
@@ -1819,7 +1819,7 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>40</v>
@@ -1828,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="5">
         <v>20438</v>
@@ -1848,7 +1848,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>40</v>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="5">
         <v>20438</v>
@@ -1883,7 +1883,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>40</v>
@@ -1891,13 +1891,15 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
       <c r="F31" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1905,7 +1907,7 @@
         <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>40</v>
@@ -1913,37 +1915,18 @@
       <c r="D32" s="5">
         <v>1</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5">
-        <v>950</v>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="H34" s="14"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="H33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>